<commit_message>
System load method modification changes
</commit_message>
<xml_diff>
--- a/Test Data/TC_135_Verify_Isolator_Units_Calculation_With_Loop_Having_Line_Isolator_Devices.xlsx
+++ b/Test Data/TC_135_Verify_Isolator_Units_Calculation_With_Loop_Having_Line_Isolator_Devices.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jdhakaa\Documents\NG Consys Project\Testing\NGConsys Automation\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D809536C-5B91-464D-B68D-1B76117F5B8E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Add Devices" sheetId="6" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="8" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="43">
   <si>
     <t>Device</t>
   </si>
@@ -158,12 +157,15 @@
   </si>
   <si>
     <t>NGC-549/TC-135</t>
+  </si>
+  <si>
+    <t>LoadingDetail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -220,7 +222,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -280,11 +282,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -325,6 +338,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -605,11 +622,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F9" sqref="F9:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -747,6 +764,9 @@
       <c r="E7" s="5" t="s">
         <v>22</v>
       </c>
+      <c r="F7" s="19" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
@@ -764,6 +784,9 @@
       <c r="E8" s="11">
         <v>6</v>
       </c>
+      <c r="F8" s="20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
@@ -781,6 +804,9 @@
       <c r="E9" s="11">
         <v>8.5</v>
       </c>
+      <c r="F9" s="20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
@@ -798,6 +824,9 @@
       <c r="E10" s="11">
         <v>9.5</v>
       </c>
+      <c r="F10" s="20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
@@ -815,6 +844,9 @@
       <c r="E11" s="11">
         <v>9.5</v>
       </c>
+      <c r="F11" s="20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
@@ -832,6 +864,9 @@
       <c r="E12" s="11">
         <v>14.5</v>
       </c>
+      <c r="F12" s="20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
@@ -849,6 +884,9 @@
       <c r="E13" s="11">
         <v>19.5</v>
       </c>
+      <c r="F13" s="20" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
@@ -865,6 +903,9 @@
       </c>
       <c r="E14" s="11">
         <v>21</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -878,7 +919,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0BBD498-A94B-42E1-9A81-1E4395982E0C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1140,5 +1181,6 @@
     <mergeCell ref="J1:K2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>